<commit_message>
fix by "Supplementary Explanation"
</commit_message>
<xml_diff>
--- a/dolphintwo/evidence.xlsx
+++ b/dolphintwo/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dd/Documents/hashquark/devops/0TODO/gon-evidence/dolphintwo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{368C506A-2FF9-9D4E-BD70-E5598EFF2AC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16645ED4-7BDA-014C-961E-5D22ED283884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="-18680" windowWidth="26220" windowHeight="13620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3800" yWindow="-19600" windowWidth="26220" windowHeight="13620" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="56">
   <si>
     <t>TxHash</t>
   </si>
@@ -193,13 +193,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>class_id</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/ddnft</t>
-  </si>
-  <si>
     <t>ddn5</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -214,9 +207,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>denom_id</t>
-  </si>
-  <si>
     <t>C48D8C36733533D59D2F3DF5F0B8BE995CA84D62858A91FA995C62AA4BCFC720</t>
   </si>
   <si>
@@ -224,13 +214,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>gon-irishub-1</t>
-  </si>
-  <si>
-    <t>gon-irishub-1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>58CC4B9CD6ACB52D81D724FD58A7A805C277392E5421C2400D9AC7854A11A804</t>
   </si>
   <si>
@@ -244,6 +227,9 @@
   <si>
     <t>D09921292D93272BB3FDD55598EDF36D051C0A6FC5E65536F1C158266FA36AED</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>elgafar-1</t>
   </si>
 </sst>
 </file>
@@ -1503,13 +1489,13 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1523,10 +1509,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1556,7 +1542,7 @@
         <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>35</v>
@@ -1570,7 +1556,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>42</v>
@@ -1588,14 +1574,6 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="E5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>46</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1609,8 +1587,8 @@
   </sheetPr>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1636,30 +1614,30 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
+        <v>54</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:8">
@@ -1669,12 +1647,8 @@
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="E5" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>49</v>
-      </c>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
@@ -1692,7 +1666,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1718,10 +1692,10 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>42</v>
@@ -1743,7 +1717,7 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -1771,16 +1745,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Evidence Format (stage-1)
</commit_message>
<xml_diff>
--- a/dolphintwo/evidence.xlsx
+++ b/dolphintwo/evidence.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dd/Documents/hashquark/devops/0TODO/gon-evidence/dolphintwo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D630201-67E5-BA48-A573-A7F403CF53D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E070AB28-C95D-DC4B-A69C-4C70937286EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="29280" windowHeight="18880" firstSheet="7" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="29280" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="99">
   <si>
     <t>TxHash</t>
   </si>
@@ -159,13 +159,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Contract-Addr</t>
-  </si>
-  <si>
-    <t>D73CEE9720E917FE910A46A2C0949EC540ADD2137F6C5A2B368DCE9A2DA30641</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ddn3</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -174,254 +167,246 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>ddn5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+  </si>
+  <si>
+    <t>ibc/80F44B622197B3F4CF25D1D7510A7F5BA50B3BBFC9DCA9B7659FB6572103BFB5</t>
+  </si>
+  <si>
+    <t>ddn6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C48D8C36733533D59D2F3DF5F0B8BE995CA84D62858A91FA995C62AA4BCFC720</t>
+  </si>
+  <si>
+    <t>58CC4B9CD6ACB52D81D724FD58A7A805C277392E5421C2400D9AC7854A11A804</t>
+  </si>
+  <si>
+    <t>B3AA3EEC0916BAD756B42075F1BC3D57443F1D0A160313B6B0806DA5A48E1F17</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D09921292D93272BB3FDD55598EDF36D051C0A6FC5E65536F1C158266FA36AED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>elgafar-1</t>
+  </si>
+  <si>
+    <t>ibc/642A6D4A68C482278B7EB54AAED7C32E376187F8997F020C0FE0F50C8D473CA9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddnftP2A7</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/DB95E45BE40C85728461C733774FB7286BA4C171843FBA7EAE893B917012CC70</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddnftP2A8</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/45C624656EE111704905A4ABE80AA53DBA7FFAA6C9026E0E3F8009CF489E778C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddnftP2A9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/3BA51B8E7E951E47B8D79BF7FE16340AA1A1DA8CD6433810F5128583C536C15A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddnftP2A10</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/B4881A9C3C2E59CE5C6E100E007E24BB348139C7223D7128E71F9F18AB57DA4F</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddnftP2A11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ibc/81491985C391BFB9F149F95CD7C221BA9511E3FB0EE74918C965DB013393B0CD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ddnftP2A12</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B842620DAE04680C8A42F7E6386BA96B6ED52A396525C140587A3EEEBCF21978</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6F9B5FD695C3F6D576FAF2A9DFEEF0390D4FE7D661A1549B8A61BA0027DB2FFA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>6E0F6AB730C01847091621D1305199712C8BA9C95DC8EDEE1FCF145E155BD40F</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2EA8098788AD0D55D0E6149E8A2B9135EDDE14A392B8EE022419D26A5AADC0FD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>689ADA5CC09A51A02D9A00A1D459A9A8EFED1DE12F77915165AA19C6F7C370A3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A0F78C0C8B481B0BAD25E5CD084FFCC47382E700B50E5F9EDFBC3ED3D70B090A</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>14F3DF23FA69A4514193D83551236BA39A7B1C8436D70A1EDEA9059010E0AB78</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>135565E5BDA54ACABD5BE71FE45F121F470DCEC2C85A60125A45F7A777A0011E</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>D02605FC62FEC268B046318CA63C6FA335670FA544A84B4B66085F35F71439A5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B92BD9B650895C0865242D26054275BE8B614DC7B2EE2C3F3104BDADA8C7EDF5</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EEA8D18E513C023DC50A49A759F53239B8E814D28548A49173EC38C5C74C3C72</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>85B05A508B7C1180DCA00DEA98E31457CD98E64D12E1E280B05017A16DC0828E</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>36B84832F23D2EC90118D529CF56D662C02BBEB318DE4BD8F60A7A72AAA7934E</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>4EF1180906473294BF83A9FF635116CA0200740EB3B5C2E943971A20906F1D0E</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>00E781D5028497AFECEEDA4BF4EBFC17581EE9E84CD92D418FB8F8D286F741EE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EB77880EF909B565980A4436C09C9837874464C74E3F386F27084CAC63319C9B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BE15DCF42F6528940014C89FF0E93900B80DE96CDFCC233DF0B0EE075F015BFC</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CE49BE5286F2C13E53965173EB71043CA67000C2DCAB4D72BDC1B145FB1CF040</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1F2081436AA987BA20655AF12707B07140C59BBDD4B81DDABBEE4C9315E72090</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>EBD5C23AD64D2C81B748973FEA7BE24088451CD6E425A08FF7B2CA3E40A548EE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>3560B5E205A0187DC1D1CC63C1ECB5F160189FED80F69CF022A748D422920A0E</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>03F87232E2CC13FBCE08DAD39BB35071EA1F368FE5FE03CCAB8F2FF0048DFA86</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>0DD877067EA5B69B2EAD0EAE2B8541104B9913C1270EDF3E26E1D4FA65846131</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>516B266DECE6C09B7B31D5DECF7816AA529F5C9B074B5071296767BFEBA7C5C9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1CF7530E01CB9998AF0A86C258921ED9EA32FA5961603F1B7717A54DDB776684</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>9E37239AFE81ED62361DD4EBF5C6E8FDF190FF53D8D636E6BDC545898F092CED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>52860E1893122A616CA0FDE2D2D6EC668AA7FA7D5EB0FFAEA87633636601953B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CA256843D9F9A9B90151AA17457E88C1050ABF49A14AF280C28E00AA802AA580</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>B88ED3DB0C34BDA3957E3CB2729F41D16314CDB0594D66BA1413E1676878049E</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>434B9E43DBC7EA4E68E117D499B831AA909B777BF5D6BF645CFB66573B3E2FBD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A44445A2140C14EA07CA1193E085DBD6EE2F7476FB896294F5A9C607BCC02252</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>97AD706138381DB0C30E7F998C4F3F54359156C8E40B7C605BD84105079771EA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>916A5DAB2E36C7B3A0E381BC146A3780A335F177F2CE215DDA681E6EFFBFE912</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>79A4C426A0E050AD0679449634FBBC97BC9ED0B6E7CF33232061482311D1B769</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gon-irishub-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uni-6</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>84F4AD97B49ADC3C21C0EDC1ED4616CA8E887489C2CDA9470558F095AE2DC666</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>gon-flixnet-1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>077DBAFE7D34E3B0D177F3D5B4389D1FFF7370B4DAAED61ED0A232A5114A421B</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t>stars1yqfl74853330krw82ye99uxacrdp8x9267t0wkd8jk2y7l7y7r2qj9hm2e</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ddn5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gon-flixnet-1</t>
-  </si>
-  <si>
-    <t>ibc/80F44B622197B3F4CF25D1D7510A7F5BA50B3BBFC9DCA9B7659FB6572103BFB5</t>
-  </si>
-  <si>
-    <t>ddn6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>C48D8C36733533D59D2F3DF5F0B8BE995CA84D62858A91FA995C62AA4BCFC720</t>
-  </si>
-  <si>
-    <t>wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh/channel-207/ddnft</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>58CC4B9CD6ACB52D81D724FD58A7A805C277392E5421C2400D9AC7854A11A804</t>
-  </si>
-  <si>
-    <t>B3AA3EEC0916BAD756B42075F1BC3D57443F1D0A160313B6B0806DA5A48E1F17</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>5072A2E5551F2F117C0D71DAD5FD23289CCED87CB7846FB65FB836DA33613558</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>D09921292D93272BB3FDD55598EDF36D051C0A6FC5E65536F1C158266FA36AED</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>elgafar-1</t>
-  </si>
-  <si>
-    <t>ibc/642A6D4A68C482278B7EB54AAED7C32E376187F8997F020C0FE0F50C8D473CA9</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ddnftP2A7</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/DB95E45BE40C85728461C733774FB7286BA4C171843FBA7EAE893B917012CC70</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ddnftP2A8</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/45C624656EE111704905A4ABE80AA53DBA7FFAA6C9026E0E3F8009CF489E778C</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ddnftP2A9</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/3BA51B8E7E951E47B8D79BF7FE16340AA1A1DA8CD6433810F5128583C536C15A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ddnftP2A10</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/B4881A9C3C2E59CE5C6E100E007E24BB348139C7223D7128E71F9F18AB57DA4F</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ddnftP2A11</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ibc/81491985C391BFB9F149F95CD7C221BA9511E3FB0EE74918C965DB013393B0CD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ddnftP2A12</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>B842620DAE04680C8A42F7E6386BA96B6ED52A396525C140587A3EEEBCF21978</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>6F9B5FD695C3F6D576FAF2A9DFEEF0390D4FE7D661A1549B8A61BA0027DB2FFA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>6E0F6AB730C01847091621D1305199712C8BA9C95DC8EDEE1FCF145E155BD40F</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>2EA8098788AD0D55D0E6149E8A2B9135EDDE14A392B8EE022419D26A5AADC0FD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>689ADA5CC09A51A02D9A00A1D459A9A8EFED1DE12F77915165AA19C6F7C370A3</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A0F78C0C8B481B0BAD25E5CD084FFCC47382E700B50E5F9EDFBC3ED3D70B090A</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>14F3DF23FA69A4514193D83551236BA39A7B1C8436D70A1EDEA9059010E0AB78</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>135565E5BDA54ACABD5BE71FE45F121F470DCEC2C85A60125A45F7A777A0011E</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>D02605FC62FEC268B046318CA63C6FA335670FA544A84B4B66085F35F71439A5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>B92BD9B650895C0865242D26054275BE8B614DC7B2EE2C3F3104BDADA8C7EDF5</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EEA8D18E513C023DC50A49A759F53239B8E814D28548A49173EC38C5C74C3C72</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>85B05A508B7C1180DCA00DEA98E31457CD98E64D12E1E280B05017A16DC0828E</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>36B84832F23D2EC90118D529CF56D662C02BBEB318DE4BD8F60A7A72AAA7934E</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>4EF1180906473294BF83A9FF635116CA0200740EB3B5C2E943971A20906F1D0E</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>00E781D5028497AFECEEDA4BF4EBFC17581EE9E84CD92D418FB8F8D286F741EE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EB77880EF909B565980A4436C09C9837874464C74E3F386F27084CAC63319C9B</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>BE15DCF42F6528940014C89FF0E93900B80DE96CDFCC233DF0B0EE075F015BFC</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CE49BE5286F2C13E53965173EB71043CA67000C2DCAB4D72BDC1B145FB1CF040</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1F2081436AA987BA20655AF12707B07140C59BBDD4B81DDABBEE4C9315E72090</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>EBD5C23AD64D2C81B748973FEA7BE24088451CD6E425A08FF7B2CA3E40A548EE</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>3560B5E205A0187DC1D1CC63C1ECB5F160189FED80F69CF022A748D422920A0E</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>03F87232E2CC13FBCE08DAD39BB35071EA1F368FE5FE03CCAB8F2FF0048DFA86</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0DD877067EA5B69B2EAD0EAE2B8541104B9913C1270EDF3E26E1D4FA65846131</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>516B266DECE6C09B7B31D5DECF7816AA529F5C9B074B5071296767BFEBA7C5C9</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1CF7530E01CB9998AF0A86C258921ED9EA32FA5961603F1B7717A54DDB776684</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>9E37239AFE81ED62361DD4EBF5C6E8FDF190FF53D8D636E6BDC545898F092CED</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>52860E1893122A616CA0FDE2D2D6EC668AA7FA7D5EB0FFAEA87633636601953B</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>CA256843D9F9A9B90151AA17457E88C1050ABF49A14AF280C28E00AA802AA580</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>B88ED3DB0C34BDA3957E3CB2729F41D16314CDB0594D66BA1413E1676878049E</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>434B9E43DBC7EA4E68E117D499B831AA909B777BF5D6BF645CFB66573B3E2FBD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A44445A2140C14EA07CA1193E085DBD6EE2F7476FB896294F5A9C607BCC02252</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>97AD706138381DB0C30E7F998C4F3F54359156C8E40B7C605BD84105079771EA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>916A5DAB2E36C7B3A0E381BC146A3780A335F177F2CE215DDA681E6EFFBFE912</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>79A4C426A0E050AD0679449634FBBC97BC9ED0B6E7CF33232061482311D1B769</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gon-irishub-1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>uni-6</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>uptick_7000-2</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>84F4AD97B49ADC3C21C0EDC1ED4616CA8E887489C2CDA9470558F095AE2DC666</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>gon-flixnet-1</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>077DBAFE7D34E3B0D177F3D5B4389D1FFF7370B4DAAED61ED0A232A5114A421B</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -824,8 +809,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -922,10 +907,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -961,10 +946,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1000,10 +985,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1039,10 +1024,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1078,34 +1063,34 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1145,37 +1130,37 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -1222,37 +1207,37 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -1294,37 +1279,37 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -1366,37 +1351,37 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -1448,37 +1433,37 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C5" s="2"/>
     </row>
@@ -1563,55 +1548,55 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -1633,7 +1618,7 @@
   </sheetPr>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -1653,60 +1638,60 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="17.25" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:4" ht="17.25" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -1960,13 +1945,13 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1980,10 +1965,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1994,7 +1979,7 @@
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="17.25" customHeight="1">
+    <row r="1" spans="1:5" ht="17.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2008,42 +1993,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17.25" customHeight="1">
+    <row r="2" spans="1:5" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>45</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:5">
       <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
+      <c r="E4" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2059,7 +2031,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:I5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2085,31 +2057,23 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>41</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2"/>
@@ -2137,7 +2101,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -2163,16 +2127,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2216,16 +2180,16 @@
     </row>
     <row r="2" spans="1:4" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2261,10 +2225,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2300,10 +2264,10 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>